<commit_message>
raw .txt changing naming convenction (only lecturers this time)
</commit_message>
<xml_diff>
--- a/transcription_app/ulrs_transcription_list.xlsx
+++ b/transcription_app/ulrs_transcription_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adriannykiel/Library/Mobile Documents/com~apple~CloudDocs/Projects/video_transciption/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E30D5CF-E4AB-DA40-BC94-483DC610487D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAC809C2-BC52-D049-9BAB-8142FF69335E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="860" windowWidth="34200" windowHeight="21380" xr2:uid="{82986ED5-21B4-284C-91F6-D5DA2E197B71}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="34200" windowHeight="20120" xr2:uid="{82986ED5-21B4-284C-91F6-D5DA2E197B71}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -728,10 +728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{872FCDE5-1B93-8B40-B54D-15E47B23FE7D}">
-  <dimension ref="A1:B57"/>
+  <dimension ref="A1:B55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+      <selection activeCell="A19" sqref="A18:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -750,311 +750,311 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>51</v>
+        <v>75</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>70</v>
+        <v>94</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>23</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>75</v>
+        <v>101</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>81</v>
+        <v>53</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>83</v>
+        <v>55</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>84</v>
+        <v>56</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>85</v>
+        <v>57</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>86</v>
+        <v>58</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>87</v>
+        <v>59</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>88</v>
+        <v>60</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>12</v>
@@ -1062,106 +1062,106 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>89</v>
+        <v>61</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>38</v>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>93</v>
+        <v>67</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>94</v>
+        <v>68</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>99</v>
+        <v>73</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>